<commit_message>
Criação da Classe dia da Semana e Script Inicial
Criação da classe para os dias da semana e alteração do script inicial
para criar as tabelas estáticas.
</commit_message>
<xml_diff>
--- a/Análise/Documentação.xlsx
+++ b/Análise/Documentação.xlsx
@@ -15,12 +15,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId1"/>
     <sheet name="Plan3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Tabela de Tipos de Pessoas</t>
   </si>
@@ -29,6 +29,30 @@
   </si>
   <si>
     <t>Jurídica</t>
+  </si>
+  <si>
+    <t>Tabela de Dia da Semana</t>
+  </si>
+  <si>
+    <t>Segunda-feira</t>
+  </si>
+  <si>
+    <t>Terça-feira</t>
+  </si>
+  <si>
+    <t>Quarta-feira</t>
+  </si>
+  <si>
+    <t>Quinta-feira</t>
+  </si>
+  <si>
+    <t>Sexta-feira</t>
+  </si>
+  <si>
+    <t>Sábado</t>
+  </si>
+  <si>
+    <t>Domingo</t>
   </si>
 </sst>
 </file>
@@ -359,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="A6:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,9 +418,72 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>